<commit_message>
Updated BOM to added AvionicsCover to the Part List
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - BOM.xlsx
+++ b/Design/CAD/mAEWing1 - BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8805" tabRatio="703" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8805" tabRatio="703" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="20" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1461" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="564">
   <si>
     <t>Description</t>
   </si>
@@ -1717,6 +1717,12 @@
   </si>
   <si>
     <t>15 pin Input Port</t>
+  </si>
+  <si>
+    <t>AvionicsCover</t>
+  </si>
+  <si>
+    <t>3D Printed part</t>
   </si>
 </sst>
 </file>
@@ -2493,10 +2499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q91"/>
+  <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2645,7 +2651,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="41" t="str">
-        <f t="shared" ref="G3:L42" si="1">IF(G$1=$F3, "X", "")</f>
+        <f t="shared" ref="G3:L43" si="1">IF(G$1=$F3, "X", "")</f>
         <v/>
       </c>
       <c r="H3" s="41" t="str">
@@ -2791,7 +2797,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="9" t="str">
-        <f t="shared" ref="E6:E31" si="3">A6&amp;"_"&amp;C6&amp;B6&amp;"_"&amp;D6</f>
+        <f t="shared" ref="E6:E32" si="3">A6&amp;"_"&amp;C6&amp;B6&amp;"_"&amp;D6</f>
         <v>mAE1_A2100_A</v>
       </c>
       <c r="F6" s="2">
@@ -4153,22 +4159,18 @@
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="7">
-        <v>2171</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>2172</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="9" t="str">
         <f t="shared" si="3"/>
-        <v>mAE1_P2171_A</v>
+        <v>mAE1_2172_</v>
       </c>
       <c r="F31" s="4">
         <v>3</v>
@@ -4198,27 +4200,35 @@
         <v/>
       </c>
       <c r="M31" s="4" t="s">
-        <v>175</v>
+        <v>562</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2">
         <v>1</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q31" s="2"/>
+        <v>464</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B32" s="7">
+        <v>2171</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E32" s="9" t="str">
-        <f t="shared" ref="E32:E33" si="5">A32&amp;"_"&amp;C32&amp;B32&amp;"_"&amp;D32</f>
-        <v>dum__</v>
+        <f t="shared" si="3"/>
+        <v>mAE1_P2171_A</v>
       </c>
       <c r="F32" s="4">
         <v>3</v>
@@ -4248,18 +4258,16 @@
         <v/>
       </c>
       <c r="M32" s="4" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2">
         <v>1</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>215</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="Q32" s="2"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
@@ -4269,7 +4277,7 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="9" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="E33:E34" si="5">A33&amp;"_"&amp;C33&amp;B33&amp;"_"&amp;D33</f>
         <v>dum__</v>
       </c>
       <c r="F33" s="4">
@@ -4300,7 +4308,7 @@
         <v/>
       </c>
       <c r="M33" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2">
@@ -4315,22 +4323,16 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="7">
-        <v>2180</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="9" t="str">
-        <f t="shared" ref="E34:E36" si="6">A34&amp;"_"&amp;C34&amp;B34&amp;"_"&amp;D34</f>
-        <v>mAE1_A2180_A</v>
-      </c>
-      <c r="F34" s="17">
+        <f t="shared" si="5"/>
+        <v>dum__</v>
+      </c>
+      <c r="F34" s="4">
         <v>3</v>
       </c>
       <c r="G34" s="41" t="str">
@@ -4357,37 +4359,39 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="M34" s="17" t="s">
-        <v>225</v>
+      <c r="M34" s="4" t="s">
+        <v>217</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q34" s="2"/>
+      <c r="Q34" s="2" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="7">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="9" t="str">
-        <f t="shared" si="6"/>
-        <v>mAE1_P2181_A</v>
+        <f t="shared" ref="E35:E37" si="6">A35&amp;"_"&amp;C35&amp;B35&amp;"_"&amp;D35</f>
+        <v>mAE1_A2180_A</v>
       </c>
       <c r="F35" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G35" s="41" t="str">
         <f t="shared" si="1"/>
@@ -4399,11 +4403,11 @@
       </c>
       <c r="I35" s="41" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J35" s="41" t="str">
         <f t="shared" si="1"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K35" s="41" t="str">
         <f t="shared" si="1"/>
@@ -4414,14 +4418,14 @@
         <v/>
       </c>
       <c r="M35" s="17" t="s">
-        <v>177</v>
+        <v>225</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>153</v>
+        <v>2</v>
       </c>
       <c r="Q35" s="2"/>
     </row>
@@ -4430,7 +4434,7 @@
         <v>8</v>
       </c>
       <c r="B36" s="7">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>14</v>
@@ -4440,9 +4444,9 @@
       </c>
       <c r="E36" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>mAE1_P2182_A</v>
-      </c>
-      <c r="F36" s="4">
+        <v>mAE1_P2181_A</v>
+      </c>
+      <c r="F36" s="17">
         <v>4</v>
       </c>
       <c r="G36" s="41" t="str">
@@ -4469,8 +4473,8 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="M36" s="4" t="s">
-        <v>176</v>
+      <c r="M36" s="17" t="s">
+        <v>177</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2">
@@ -4481,59 +4485,61 @@
       </c>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B37" s="7">
+        <v>2182</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E37" s="9" t="str">
-        <f>A37&amp;"_"&amp;C37&amp;B37&amp;"_"&amp;D37</f>
-        <v>dum__</v>
-      </c>
-      <c r="F37" s="2">
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>mAE1_P2182_A</v>
+      </c>
+      <c r="F37" s="4">
+        <v>4</v>
       </c>
       <c r="G37" s="41" t="str">
-        <f t="shared" ref="G37:L77" si="7">IF(G$1=$F37, "X", "")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="H37" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="I37" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="J37" s="41" t="str">
+        <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="J37" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
       <c r="K37" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="L37" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>190</v>
-      </c>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="M37" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="N37" s="2"/>
       <c r="O37" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>215</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="Q37" s="2"/>
     </row>
     <row r="38" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -4550,7 +4556,7 @@
         <v>3</v>
       </c>
       <c r="G38" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="G38:L78" si="7">IF(G$1=$F38, "X", "")</f>
         <v/>
       </c>
       <c r="H38" s="41" t="str">
@@ -4574,9 +4580,11 @@
         <v/>
       </c>
       <c r="M38" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="N38" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="O38" s="2">
         <v>2</v>
       </c>
@@ -4589,20 +4597,14 @@
     </row>
     <row r="39" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" s="7">
-        <v>2191</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
       <c r="E39" s="9" t="str">
         <f>A39&amp;"_"&amp;C39&amp;B39&amp;"_"&amp;D39</f>
-        <v>mAE1_P2191_A</v>
+        <v>dum__</v>
       </c>
       <c r="F39" s="2">
         <v>3</v>
@@ -4631,30 +4633,36 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="M39" s="4" t="s">
-        <v>463</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>494</v>
-      </c>
+      <c r="M39" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="N39" s="2"/>
       <c r="O39" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="Q39" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="40" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B40" s="7">
+        <v>2191</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E40" s="9" t="str">
         <f>A40&amp;"_"&amp;C40&amp;B40&amp;"_"&amp;D40</f>
-        <v>dum__</v>
+        <v>mAE1_P2191_A</v>
       </c>
       <c r="F40" s="2">
         <v>3</v>
@@ -4683,19 +4691,19 @@
         <f t="shared" si="7"/>
         <v/>
       </c>
-      <c r="M40" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="N40" s="2"/>
+      <c r="M40" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>494</v>
+      </c>
       <c r="O40" s="2">
         <v>1</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>215</v>
-      </c>
+        <v>464</v>
+      </c>
+      <c r="Q40" s="2"/>
     </row>
     <row r="41" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -4736,7 +4744,7 @@
         <v/>
       </c>
       <c r="M41" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2">
@@ -4749,97 +4757,93 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
+    <row r="42" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>406</v>
+      </c>
       <c r="B42" s="7"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="36" t="str">
+      <c r="E42" s="9" t="str">
+        <f>A42&amp;"_"&amp;C42&amp;B42&amp;"_"&amp;D42</f>
+        <v>dum__</v>
+      </c>
+      <c r="F42" s="2">
+        <v>3</v>
+      </c>
+      <c r="G42" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="H42" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I42" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v>X</v>
+      </c>
+      <c r="J42" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K42" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L42" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2">
+        <v>1</v>
+      </c>
+      <c r="P42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q42" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="H42" s="36" t="str">
+      <c r="H43" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I42" s="36" t="str">
+      <c r="I43" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="J42" s="36" t="str">
+      <c r="J43" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K42" s="36" t="str">
+      <c r="K43" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="L42" s="36" t="str">
+      <c r="L43" s="36" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="M42" s="4"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="7">
-        <v>2200</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E43" s="9" t="str">
-        <f t="shared" ref="E43:E57" si="8">A43&amp;"_"&amp;C43&amp;B43&amp;"_"&amp;D43</f>
-        <v>mAE1_A2200_A</v>
-      </c>
-      <c r="F43" s="2">
-        <v>2</v>
-      </c>
-      <c r="G43" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="H43" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v>X</v>
-      </c>
-      <c r="I43" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J43" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="K43" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L43" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="M43" s="4"/>
       <c r="N43" s="2"/>
-      <c r="O43" s="2">
-        <v>1</v>
-      </c>
-      <c r="P43" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -4847,7 +4851,7 @@
         <v>8</v>
       </c>
       <c r="B44" s="7">
-        <v>2210</v>
+        <v>2200</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>5</v>
@@ -4856,101 +4860,101 @@
         <v>5</v>
       </c>
       <c r="E44" s="9" t="str">
+        <f t="shared" ref="E44:E58" si="8">A44&amp;"_"&amp;C44&amp;B44&amp;"_"&amp;D44</f>
+        <v>mAE1_A2200_A</v>
+      </c>
+      <c r="F44" s="2">
+        <v>2</v>
+      </c>
+      <c r="G44" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="H44" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v>X</v>
+      </c>
+      <c r="I44" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J44" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K44" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L44" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2">
+        <v>1</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q44" s="2"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="7">
+        <v>2210</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="9" t="str">
         <f t="shared" si="8"/>
         <v>mAE1_A2210_A</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F45" s="2">
         <v>3</v>
       </c>
-      <c r="G44" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="H44" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="I44" s="41" t="str">
+      <c r="G45" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="H45" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I45" s="41" t="str">
         <f t="shared" si="7"/>
         <v>X</v>
       </c>
-      <c r="J44" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="K44" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L44" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="M44" s="2" t="s">
+      <c r="J45" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K45" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L45" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M45" s="2" t="s">
         <v>412</v>
-      </c>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2">
-        <v>1</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q44" s="2"/>
-    </row>
-    <row r="45" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="7">
-        <v>2211</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E45" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>mAE1_P2211_A</v>
-      </c>
-      <c r="F45" s="2">
-        <v>4</v>
-      </c>
-      <c r="G45" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="H45" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="I45" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J45" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v>X</v>
-      </c>
-      <c r="K45" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L45" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2">
         <v>1</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>410</v>
+        <v>188</v>
       </c>
       <c r="Q45" s="2"/>
     </row>
@@ -4959,7 +4963,7 @@
         <v>8</v>
       </c>
       <c r="B46" s="7">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>14</v>
@@ -4969,7 +4973,7 @@
       </c>
       <c r="E46" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>mAE1_P2212_A</v>
+        <v>mAE1_P2211_A</v>
       </c>
       <c r="F46" s="2">
         <v>4</v>
@@ -4999,23 +5003,23 @@
         <v/>
       </c>
       <c r="M46" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2">
         <v>1</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q46" s="2"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="7">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>14</v>
@@ -5024,45 +5028,45 @@
         <v>5</v>
       </c>
       <c r="E47" s="9" t="str">
-        <f t="shared" ref="E47:E53" si="9">A47&amp;"_"&amp;C47&amp;B47&amp;"_"&amp;D47</f>
-        <v>mAE1_P2213_A</v>
+        <f t="shared" si="8"/>
+        <v>mAE1_P2212_A</v>
       </c>
       <c r="F47" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G47" s="41" t="str">
-        <f t="shared" ref="G47:L53" si="10">IF(G$1=$F47, "X", "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H47" s="41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I47" s="41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J47" s="41" t="str">
+        <f t="shared" si="7"/>
         <v>X</v>
       </c>
-      <c r="J47" s="41" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
       <c r="K47" s="41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L47" s="41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M47" s="2" t="s">
-        <v>183</v>
+        <v>409</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2">
         <v>1</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>165</v>
+        <v>411</v>
       </c>
       <c r="Q47" s="2"/>
     </row>
@@ -5071,7 +5075,7 @@
         <v>8</v>
       </c>
       <c r="B48" s="7">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>14</v>
@@ -5080,14 +5084,14 @@
         <v>5</v>
       </c>
       <c r="E48" s="9" t="str">
-        <f t="shared" si="9"/>
-        <v>mAE1_P2214_A</v>
+        <f t="shared" ref="E48:E54" si="9">A48&amp;"_"&amp;C48&amp;B48&amp;"_"&amp;D48</f>
+        <v>mAE1_P2213_A</v>
       </c>
       <c r="F48" s="2">
         <v>3</v>
       </c>
       <c r="G48" s="41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="G48:L54" si="10">IF(G$1=$F48, "X", "")</f>
         <v/>
       </c>
       <c r="H48" s="41" t="str">
@@ -5111,7 +5115,7 @@
         <v/>
       </c>
       <c r="M48" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2">
@@ -5127,7 +5131,7 @@
         <v>8</v>
       </c>
       <c r="B49" s="7">
-        <v>2215</v>
+        <v>2214</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>14</v>
@@ -5137,7 +5141,7 @@
       </c>
       <c r="E49" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>mAE1_P2215_A</v>
+        <v>mAE1_P2214_A</v>
       </c>
       <c r="F49" s="2">
         <v>3</v>
@@ -5167,7 +5171,7 @@
         <v/>
       </c>
       <c r="M49" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2">
@@ -5183,7 +5187,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="7">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>14</v>
@@ -5193,7 +5197,7 @@
       </c>
       <c r="E50" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>mAE1_P2216_A</v>
+        <v>mAE1_P2215_A</v>
       </c>
       <c r="F50" s="2">
         <v>3</v>
@@ -5223,7 +5227,7 @@
         <v/>
       </c>
       <c r="M50" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2">
@@ -5239,7 +5243,7 @@
         <v>8</v>
       </c>
       <c r="B51" s="7">
-        <v>2220</v>
+        <v>2216</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>14</v>
@@ -5249,7 +5253,7 @@
       </c>
       <c r="E51" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>mAE1_P2220_A</v>
+        <v>mAE1_P2216_A</v>
       </c>
       <c r="F51" s="2">
         <v>3</v>
@@ -5279,14 +5283,14 @@
         <v/>
       </c>
       <c r="M51" s="2" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2">
         <v>1</v>
       </c>
       <c r="P51" s="2" t="s">
-        <v>233</v>
+        <v>165</v>
       </c>
       <c r="Q51" s="2"/>
     </row>
@@ -5295,7 +5299,7 @@
         <v>8</v>
       </c>
       <c r="B52" s="7">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>14</v>
@@ -5305,7 +5309,7 @@
       </c>
       <c r="E52" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>mAE1_P2221_A</v>
+        <v>mAE1_P2220_A</v>
       </c>
       <c r="F52" s="2">
         <v>3</v>
@@ -5335,7 +5339,7 @@
         <v/>
       </c>
       <c r="M52" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2">
@@ -5351,7 +5355,7 @@
         <v>8</v>
       </c>
       <c r="B53" s="7">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>14</v>
@@ -5361,7 +5365,7 @@
       </c>
       <c r="E53" s="9" t="str">
         <f t="shared" si="9"/>
-        <v>mAE1_P2222_A</v>
+        <v>mAE1_P2221_A</v>
       </c>
       <c r="F53" s="2">
         <v>3</v>
@@ -5391,7 +5395,7 @@
         <v/>
       </c>
       <c r="M53" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2">
@@ -5407,7 +5411,7 @@
         <v>8</v>
       </c>
       <c r="B54" s="7">
-        <v>2230</v>
+        <v>2222</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>14</v>
@@ -5416,45 +5420,45 @@
         <v>5</v>
       </c>
       <c r="E54" s="9" t="str">
-        <f t="shared" si="8"/>
-        <v>mAE1_P2230_A</v>
+        <f t="shared" si="9"/>
+        <v>mAE1_P2222_A</v>
       </c>
       <c r="F54" s="2">
         <v>3</v>
       </c>
       <c r="G54" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="H54" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="I54" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>X</v>
       </c>
       <c r="J54" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="K54" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="L54" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="M54" s="2" t="s">
-        <v>322</v>
+        <v>180</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2">
         <v>1</v>
       </c>
       <c r="P54" s="2" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
       <c r="Q54" s="2"/>
     </row>
@@ -5463,7 +5467,7 @@
         <v>8</v>
       </c>
       <c r="B55" s="7">
-        <v>2240</v>
+        <v>2230</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>14</v>
@@ -5473,7 +5477,7 @@
       </c>
       <c r="E55" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>mAE1_P2240_A</v>
+        <v>mAE1_P2230_A</v>
       </c>
       <c r="F55" s="2">
         <v>3</v>
@@ -5503,7 +5507,7 @@
         <v/>
       </c>
       <c r="M55" s="2" t="s">
-        <v>181</v>
+        <v>322</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2">
@@ -5519,7 +5523,7 @@
         <v>8</v>
       </c>
       <c r="B56" s="7">
-        <v>2250</v>
+        <v>2240</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>14</v>
@@ -5529,7 +5533,7 @@
       </c>
       <c r="E56" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>mAE1_P2250_A</v>
+        <v>mAE1_P2240_A</v>
       </c>
       <c r="F56" s="2">
         <v>3</v>
@@ -5559,7 +5563,7 @@
         <v/>
       </c>
       <c r="M56" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2">
@@ -5575,7 +5579,7 @@
         <v>8</v>
       </c>
       <c r="B57" s="7">
-        <v>2260</v>
+        <v>2250</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>14</v>
@@ -5585,7 +5589,7 @@
       </c>
       <c r="E57" s="9" t="str">
         <f t="shared" si="8"/>
-        <v>mAE1_P2260_A</v>
+        <v>mAE1_P2250_A</v>
       </c>
       <c r="F57" s="2">
         <v>3</v>
@@ -5615,29 +5619,33 @@
         <v/>
       </c>
       <c r="M57" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P57" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q57" s="2" t="s">
-        <v>305</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="Q57" s="2"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B58" s="7">
+        <v>2260</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E58" s="9" t="str">
-        <f>A58&amp;"_"&amp;C58&amp;B58&amp;"_"&amp;D58</f>
-        <v>dum__</v>
+        <f t="shared" si="8"/>
+        <v>mAE1_P2260_A</v>
       </c>
       <c r="F58" s="2">
         <v>3</v>
@@ -5667,22 +5675,20 @@
         <v/>
       </c>
       <c r="M58" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="N58" s="2" t="s">
-        <v>190</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="N58" s="2"/>
       <c r="O58" s="2">
         <v>3</v>
       </c>
       <c r="P58" s="2" t="s">
-        <v>2</v>
+        <v>233</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>406</v>
       </c>
@@ -5721,11 +5727,13 @@
         <v/>
       </c>
       <c r="M59" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="N59" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="N59" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="O59" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P59" s="2" t="s">
         <v>2</v>
@@ -5734,96 +5742,92 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
+    <row r="60" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>406</v>
+      </c>
       <c r="B60" s="7"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="36" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="H60" s="36" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="I60" s="36" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J60" s="36" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="K60" s="36" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L60" s="36" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="M60" s="2"/>
+      <c r="E60" s="9" t="str">
+        <f>A60&amp;"_"&amp;C60&amp;B60&amp;"_"&amp;D60</f>
+        <v>dum__</v>
+      </c>
+      <c r="F60" s="2">
+        <v>3</v>
+      </c>
+      <c r="G60" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="H60" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I60" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v>X</v>
+      </c>
+      <c r="J60" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K60" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L60" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>413</v>
+      </c>
       <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="2"/>
-    </row>
-    <row r="61" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B61" s="7">
-        <v>2300</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" s="9" t="str">
-        <f t="shared" ref="E61:E64" si="11">A61&amp;"_"&amp;C61&amp;B61&amp;"_"&amp;D61</f>
-        <v>mAE1_A2300_A</v>
-      </c>
-      <c r="F61" s="2">
+      <c r="O60" s="2">
         <v>2</v>
       </c>
-      <c r="G61" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="H61" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v>X</v>
-      </c>
-      <c r="I61" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J61" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="K61" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="L61" s="41" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="M61" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="P60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q60" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="36" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="H61" s="36" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I61" s="36" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J61" s="36" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K61" s="36" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L61" s="36" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M61" s="2"/>
       <c r="N61" s="2"/>
-      <c r="O61" s="2">
-        <v>1</v>
-      </c>
-      <c r="P61" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="O61" s="2"/>
+      <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
     </row>
     <row r="62" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -5831,7 +5835,7 @@
         <v>8</v>
       </c>
       <c r="B62" s="7">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>5</v>
@@ -5840,11 +5844,11 @@
         <v>5</v>
       </c>
       <c r="E62" s="9" t="str">
-        <f t="shared" si="11"/>
-        <v>mAE1_A2310_A</v>
+        <f t="shared" ref="E62:E65" si="11">A62&amp;"_"&amp;C62&amp;B62&amp;"_"&amp;D62</f>
+        <v>mAE1_A2300_A</v>
       </c>
       <c r="F62" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G62" s="41" t="str">
         <f t="shared" si="7"/>
@@ -5852,11 +5856,11 @@
       </c>
       <c r="H62" s="41" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="I62" s="41" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="J62" s="41" t="str">
         <f t="shared" si="7"/>
@@ -5871,14 +5875,14 @@
         <v/>
       </c>
       <c r="M62" s="2" t="s">
-        <v>412</v>
+        <v>15</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2">
         <v>1</v>
       </c>
       <c r="P62" s="2" t="s">
-        <v>188</v>
+        <v>2</v>
       </c>
       <c r="Q62" s="2"/>
     </row>
@@ -5887,20 +5891,20 @@
         <v>8</v>
       </c>
       <c r="B63" s="7">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E63" s="9" t="str">
         <f t="shared" si="11"/>
-        <v>mAE1_P2311_A</v>
+        <v>mAE1_A2310_A</v>
       </c>
       <c r="F63" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G63" s="41" t="str">
         <f t="shared" si="7"/>
@@ -5912,11 +5916,11 @@
       </c>
       <c r="I63" s="41" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J63" s="41" t="str">
         <f t="shared" si="7"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="K63" s="41" t="str">
         <f t="shared" si="7"/>
@@ -5927,14 +5931,14 @@
         <v/>
       </c>
       <c r="M63" s="2" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2">
         <v>1</v>
       </c>
       <c r="P63" s="2" t="s">
-        <v>410</v>
+        <v>188</v>
       </c>
       <c r="Q63" s="2"/>
     </row>
@@ -5943,7 +5947,7 @@
         <v>8</v>
       </c>
       <c r="B64" s="7">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>14</v>
@@ -5953,7 +5957,7 @@
       </c>
       <c r="E64" s="9" t="str">
         <f t="shared" si="11"/>
-        <v>mAE1_P2312_A</v>
+        <v>mAE1_P2311_A</v>
       </c>
       <c r="F64" s="2">
         <v>4</v>
@@ -5983,14 +5987,14 @@
         <v/>
       </c>
       <c r="M64" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" s="2">
         <v>1</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q64" s="2"/>
     </row>
@@ -5999,7 +6003,7 @@
         <v>8</v>
       </c>
       <c r="B65" s="7">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>14</v>
@@ -6008,45 +6012,45 @@
         <v>5</v>
       </c>
       <c r="E65" s="9" t="str">
-        <f t="shared" ref="E65:E71" si="12">A65&amp;"_"&amp;C65&amp;B65&amp;"_"&amp;D65</f>
-        <v>mAE1_P2313_A</v>
+        <f t="shared" si="11"/>
+        <v>mAE1_P2312_A</v>
       </c>
       <c r="F65" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G65" s="41" t="str">
-        <f t="shared" ref="G65:L71" si="13">IF(G$1=$F65, "X", "")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="H65" s="41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I65" s="41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="J65" s="41" t="str">
+        <f t="shared" si="7"/>
         <v>X</v>
       </c>
-      <c r="J65" s="41" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
       <c r="K65" s="41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L65" s="41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M65" s="2" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="N65" s="2"/>
       <c r="O65" s="2">
         <v>1</v>
       </c>
       <c r="P65" s="2" t="s">
-        <v>165</v>
+        <v>411</v>
       </c>
       <c r="Q65" s="2"/>
     </row>
@@ -6055,7 +6059,7 @@
         <v>8</v>
       </c>
       <c r="B66" s="7">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>14</v>
@@ -6064,14 +6068,14 @@
         <v>5</v>
       </c>
       <c r="E66" s="9" t="str">
-        <f t="shared" si="12"/>
-        <v>mAE1_P2314_A</v>
+        <f t="shared" ref="E66:E72" si="12">A66&amp;"_"&amp;C66&amp;B66&amp;"_"&amp;D66</f>
+        <v>mAE1_P2313_A</v>
       </c>
       <c r="F66" s="2">
         <v>3</v>
       </c>
       <c r="G66" s="41" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="G66:L72" si="13">IF(G$1=$F66, "X", "")</f>
         <v/>
       </c>
       <c r="H66" s="41" t="str">
@@ -6095,7 +6099,7 @@
         <v/>
       </c>
       <c r="M66" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2">
@@ -6111,7 +6115,7 @@
         <v>8</v>
       </c>
       <c r="B67" s="7">
-        <v>2315</v>
+        <v>2314</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>14</v>
@@ -6121,7 +6125,7 @@
       </c>
       <c r="E67" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>mAE1_P2315_A</v>
+        <v>mAE1_P2314_A</v>
       </c>
       <c r="F67" s="2">
         <v>3</v>
@@ -6151,7 +6155,7 @@
         <v/>
       </c>
       <c r="M67" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" s="2">
@@ -6167,7 +6171,7 @@
         <v>8</v>
       </c>
       <c r="B68" s="7">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>14</v>
@@ -6177,7 +6181,7 @@
       </c>
       <c r="E68" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>mAE1_P2316_A</v>
+        <v>mAE1_P2315_A</v>
       </c>
       <c r="F68" s="2">
         <v>3</v>
@@ -6207,7 +6211,7 @@
         <v/>
       </c>
       <c r="M68" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2">
@@ -6223,7 +6227,7 @@
         <v>8</v>
       </c>
       <c r="B69" s="7">
-        <v>2320</v>
+        <v>2316</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>14</v>
@@ -6233,7 +6237,7 @@
       </c>
       <c r="E69" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>mAE1_P2320_A</v>
+        <v>mAE1_P2316_A</v>
       </c>
       <c r="F69" s="2">
         <v>3</v>
@@ -6263,14 +6267,14 @@
         <v/>
       </c>
       <c r="M69" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2">
         <v>1</v>
       </c>
       <c r="P69" s="2" t="s">
-        <v>233</v>
+        <v>165</v>
       </c>
       <c r="Q69" s="2"/>
     </row>
@@ -6279,7 +6283,7 @@
         <v>8</v>
       </c>
       <c r="B70" s="7">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>14</v>
@@ -6289,7 +6293,7 @@
       </c>
       <c r="E70" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>mAE1_P2321_A</v>
+        <v>mAE1_P2320_A</v>
       </c>
       <c r="F70" s="2">
         <v>3</v>
@@ -6319,7 +6323,7 @@
         <v/>
       </c>
       <c r="M70" s="2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" s="2">
@@ -6335,7 +6339,7 @@
         <v>8</v>
       </c>
       <c r="B71" s="7">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>14</v>
@@ -6345,7 +6349,7 @@
       </c>
       <c r="E71" s="9" t="str">
         <f t="shared" si="12"/>
-        <v>mAE1_P2322_A</v>
+        <v>mAE1_P2321_A</v>
       </c>
       <c r="F71" s="2">
         <v>3</v>
@@ -6375,7 +6379,7 @@
         <v/>
       </c>
       <c r="M71" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" s="2">
@@ -6391,7 +6395,7 @@
         <v>8</v>
       </c>
       <c r="B72" s="7">
-        <v>2330</v>
+        <v>2322</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>14</v>
@@ -6400,45 +6404,45 @@
         <v>5</v>
       </c>
       <c r="E72" s="9" t="str">
-        <f t="shared" ref="E72:E75" si="14">A72&amp;"_"&amp;C72&amp;B72&amp;"_"&amp;D72</f>
-        <v>mAE1_P2330_A</v>
+        <f t="shared" si="12"/>
+        <v>mAE1_P2322_A</v>
       </c>
       <c r="F72" s="2">
         <v>3</v>
       </c>
       <c r="G72" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="H72" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="I72" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>X</v>
       </c>
       <c r="J72" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="K72" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="L72" s="41" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="M72" s="2" t="s">
-        <v>322</v>
+        <v>420</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" s="2">
         <v>1</v>
       </c>
       <c r="P72" s="2" t="s">
-        <v>158</v>
+        <v>233</v>
       </c>
       <c r="Q72" s="2"/>
     </row>
@@ -6447,7 +6451,7 @@
         <v>8</v>
       </c>
       <c r="B73" s="7">
-        <v>2340</v>
+        <v>2330</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>14</v>
@@ -6456,8 +6460,8 @@
         <v>5</v>
       </c>
       <c r="E73" s="9" t="str">
-        <f t="shared" si="14"/>
-        <v>mAE1_P2340_A</v>
+        <f t="shared" ref="E73:E76" si="14">A73&amp;"_"&amp;C73&amp;B73&amp;"_"&amp;D73</f>
+        <v>mAE1_P2330_A</v>
       </c>
       <c r="F73" s="2">
         <v>3</v>
@@ -6487,7 +6491,7 @@
         <v/>
       </c>
       <c r="M73" s="2" t="s">
-        <v>181</v>
+        <v>322</v>
       </c>
       <c r="N73" s="2"/>
       <c r="O73" s="2">
@@ -6503,7 +6507,7 @@
         <v>8</v>
       </c>
       <c r="B74" s="7">
-        <v>2350</v>
+        <v>2340</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>14</v>
@@ -6513,7 +6517,7 @@
       </c>
       <c r="E74" s="9" t="str">
         <f t="shared" si="14"/>
-        <v>mAE1_P2350_A</v>
+        <v>mAE1_P2340_A</v>
       </c>
       <c r="F74" s="2">
         <v>3</v>
@@ -6543,7 +6547,7 @@
         <v/>
       </c>
       <c r="M74" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" s="2">
@@ -6559,7 +6563,7 @@
         <v>8</v>
       </c>
       <c r="B75" s="7">
-        <v>2360</v>
+        <v>2350</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>14</v>
@@ -6569,7 +6573,7 @@
       </c>
       <c r="E75" s="9" t="str">
         <f t="shared" si="14"/>
-        <v>mAE1_P2360_A</v>
+        <v>mAE1_P2350_A</v>
       </c>
       <c r="F75" s="2">
         <v>3</v>
@@ -6599,29 +6603,33 @@
         <v/>
       </c>
       <c r="M75" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="Q75" s="2" t="s">
-        <v>305</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="Q75" s="2"/>
     </row>
     <row r="76" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>406</v>
-      </c>
-      <c r="B76" s="7"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="B76" s="7">
+        <v>2360</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E76" s="9" t="str">
-        <f>A76&amp;"_"&amp;C76&amp;B76&amp;"_"&amp;D76</f>
-        <v>dum__</v>
+        <f t="shared" si="14"/>
+        <v>mAE1_P2360_A</v>
       </c>
       <c r="F76" s="2">
         <v>3</v>
@@ -6651,19 +6659,17 @@
         <v/>
       </c>
       <c r="M76" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="N76" s="2" t="s">
-        <v>190</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="N76" s="2"/>
       <c r="O76" s="2">
         <v>3</v>
       </c>
       <c r="P76" s="2" t="s">
-        <v>2</v>
+        <v>233</v>
       </c>
       <c r="Q76" s="2" t="s">
-        <v>215</v>
+        <v>305</v>
       </c>
     </row>
     <row r="77" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
@@ -6705,11 +6711,13 @@
         <v/>
       </c>
       <c r="M77" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="N77" s="2"/>
+        <v>172</v>
+      </c>
+      <c r="N77" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="O77" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P77" s="2" t="s">
         <v>2</v>
@@ -6718,40 +6726,69 @@
         <v>215</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A80" s="38" t="s">
+    <row r="78" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="B78" s="7"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="9" t="str">
+        <f>A78&amp;"_"&amp;C78&amp;B78&amp;"_"&amp;D78</f>
+        <v>dum__</v>
+      </c>
+      <c r="F78" s="2">
+        <v>3</v>
+      </c>
+      <c r="G78" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="H78" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="I78" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v>X</v>
+      </c>
+      <c r="J78" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="K78" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="L78" s="41" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="M78" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="N78" s="2"/>
+      <c r="O78" s="2">
+        <v>2</v>
+      </c>
+      <c r="P78" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q78" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A81" s="38" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>7</v>
-      </c>
-      <c r="B81" s="53" t="s">
-        <v>407</v>
-      </c>
-      <c r="C81" s="53"/>
-      <c r="D81" s="53"/>
-      <c r="E81" s="53"/>
-      <c r="F81" s="53"/>
-      <c r="G81" s="53"/>
-      <c r="H81" s="53"/>
-      <c r="I81" s="53"/>
-      <c r="J81" s="53"/>
-      <c r="K81" s="53"/>
-      <c r="L81" s="53"/>
-      <c r="M81" s="53"/>
-      <c r="N81" s="53"/>
-      <c r="O81" s="53"/>
-      <c r="P81" s="53"/>
-      <c r="Q81" s="53"/>
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B82" s="53" t="s">
-        <v>324</v>
+        <v>407</v>
       </c>
       <c r="C82" s="53"/>
       <c r="D82" s="53"/>
@@ -6771,10 +6808,10 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B83" s="53" t="s">
-        <v>404</v>
+        <v>324</v>
       </c>
       <c r="C83" s="53"/>
       <c r="D83" s="53"/>
@@ -6794,10 +6831,10 @@
     </row>
     <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B84" s="53" t="s">
-        <v>325</v>
+        <v>404</v>
       </c>
       <c r="C84" s="53"/>
       <c r="D84" s="53"/>
@@ -6817,10 +6854,10 @@
     </row>
     <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B85" s="53" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C85" s="53"/>
       <c r="D85" s="53"/>
@@ -6840,10 +6877,10 @@
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>321</v>
+        <v>9</v>
       </c>
       <c r="B86" s="53" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C86" s="53"/>
       <c r="D86" s="53"/>
@@ -6863,10 +6900,10 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="B87" s="53" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C87" s="53"/>
       <c r="D87" s="53"/>
@@ -6886,10 +6923,10 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B88" s="53" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C88" s="53"/>
       <c r="D88" s="53"/>
@@ -6909,10 +6946,10 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>18</v>
+        <v>329</v>
       </c>
       <c r="B89" s="53" t="s">
-        <v>405</v>
+        <v>329</v>
       </c>
       <c r="C89" s="53"/>
       <c r="D89" s="53"/>
@@ -6932,10 +6969,10 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B90" s="53" t="s">
-        <v>330</v>
+        <v>405</v>
       </c>
       <c r="C90" s="53"/>
       <c r="D90" s="53"/>
@@ -6955,10 +6992,10 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B91" s="53" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C91" s="53"/>
       <c r="D91" s="53"/>
@@ -6976,19 +7013,42 @@
       <c r="P91" s="53"/>
       <c r="Q91" s="53"/>
     </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="53" t="s">
+        <v>331</v>
+      </c>
+      <c r="C92" s="53"/>
+      <c r="D92" s="53"/>
+      <c r="E92" s="53"/>
+      <c r="F92" s="53"/>
+      <c r="G92" s="53"/>
+      <c r="H92" s="53"/>
+      <c r="I92" s="53"/>
+      <c r="J92" s="53"/>
+      <c r="K92" s="53"/>
+      <c r="L92" s="53"/>
+      <c r="M92" s="53"/>
+      <c r="N92" s="53"/>
+      <c r="O92" s="53"/>
+      <c r="P92" s="53"/>
+      <c r="Q92" s="53"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B91:Q91"/>
+    <mergeCell ref="B82:Q82"/>
+    <mergeCell ref="B83:Q83"/>
+    <mergeCell ref="B84:Q84"/>
+    <mergeCell ref="B85:Q85"/>
     <mergeCell ref="B86:Q86"/>
+    <mergeCell ref="B92:Q92"/>
     <mergeCell ref="B87:Q87"/>
     <mergeCell ref="B88:Q88"/>
     <mergeCell ref="B89:Q89"/>
     <mergeCell ref="B90:Q90"/>
-    <mergeCell ref="B81:Q81"/>
-    <mergeCell ref="B82:Q82"/>
-    <mergeCell ref="B83:Q83"/>
-    <mergeCell ref="B84:Q84"/>
-    <mergeCell ref="B85:Q85"/>
+    <mergeCell ref="B91:Q91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6999,7 +7059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
     </sheetView>

</xml_diff>